<commit_message>
fixed ticketBuilderRevisedEdition and other stuff
</commit_message>
<xml_diff>
--- a/stockWinnersFromAIStockPicker.xlsx
+++ b/stockWinnersFromAIStockPicker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,17 +441,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>class40</t>
+          <t>class</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>986</v>
+        <v>4159</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>MAA</t>
+          <t>XBIT</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -460,11 +460,11 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>1103</v>
+        <v>12709</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TGTX</t>
+          <t>ICCT</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -473,93 +473,15 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>1679</v>
+        <v>12779</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>CIB</t>
+          <t>LCLP</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>1749</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>BOH</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>1995</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>CLSD</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
-        <v>2050</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>HASI</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>2164</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>AVAL</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>2171</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>SKY</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="1" t="n">
-        <v>2383</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>NYMX</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>